<commit_message>
Add Google Search function
</commit_message>
<xml_diff>
--- a/data/Intents.xlsx
+++ b/data/Intents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code and money\11.11 chatbot\chatbot_my_1\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/houyixin/COMP3074_CW/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCEE990-95AA-4153-BB7B-6E8BCC336FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4432058F-9597-4B46-BD02-6CBB0500090D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intents" sheetId="1" r:id="rId1"/>
@@ -66,10 +66,6 @@
     <t>I can assist you with booking a table and answer questions., Type 'book' to make a reservation or ask me anything and I’ll do my best to answer!</t>
   </si>
   <si>
-    <t>thank you, thanks, I appreciate it</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>how are you, how's it going, how are you feeling, how’s your day</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -86,10 +82,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>what's up, what’s happening, what’s new</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Not much just waiting to assist you!, Just here and ready to help!, I’m here feel free to ask me anything!</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -112,20 +104,24 @@
     <t>negative_responses</t>
   </si>
   <si>
-    <t>yes, y, okay, confirm,ok</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Glad to be of assistance!</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>no, n, nu</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>I am sorry for that</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>n, no, nah, nope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y, yes, okay, confirm, ok, yeah, sure </t>
+  </si>
+  <si>
+    <t>thank you, thanks, I appreciate it</t>
+  </si>
+  <si>
+    <t>what's up, what’s happening, what’s new, whats up</t>
   </si>
 </sst>
 </file>
@@ -136,7 +132,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -144,7 +140,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -152,7 +148,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="等线 Light"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -161,7 +157,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -170,7 +166,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -179,7 +175,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -187,7 +183,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -195,7 +191,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -203,7 +199,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -211,7 +207,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -220,7 +216,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -229,7 +225,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -237,7 +233,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -246,7 +242,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -254,7 +250,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -263,7 +259,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -272,7 +268,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -280,14 +276,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -725,48 +721,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -782,9 +778,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -822,7 +818,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -928,7 +924,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1070,7 +1066,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1080,15 +1076,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="256" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.25" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="54.5" customWidth="1"/>
-    <col min="3" max="3" width="206.125" customWidth="1"/>
+    <col min="3" max="3" width="206.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1110,7 +1106,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1129,10 +1125,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1140,10 +1136,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1151,7 +1147,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -1162,10 +1158,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1173,32 +1169,32 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add save history function
</commit_message>
<xml_diff>
--- a/data/Intents.xlsx
+++ b/data/Intents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/houyixin/COMP3074_CW/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439D1C63-5281-A744-BDBF-7332DBE1390A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D8BAF5-5596-4D4C-9ECF-F37BF972A5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>exit</t>
   </si>
@@ -127,13 +127,19 @@
     <t>name</t>
   </si>
   <si>
-    <t>do you remember my name, do you know my name, who am i, tell me who am i, call my name, what's my name, call me</t>
-  </si>
-  <si>
     <t>change</t>
   </si>
   <si>
     <t>change, change my name, update, update my name</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>time, current time, what time is it, can you tell me the time, do you know the current time</t>
+  </si>
+  <si>
+    <t>my name, do you remember my name, do you know my name, who am i, tell me who am i, call my name, what's my name, call me, my name is</t>
   </si>
 </sst>
 </file>
@@ -1086,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="256" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="256" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1214,15 +1220,23 @@
         <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add all new stuff
</commit_message>
<xml_diff>
--- a/data/Intents.xlsx
+++ b/data/Intents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/houyixin/COMP3074_CW/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code and money\11.11 chatbot\12.4 chatbot\COMP3074_CW-main\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D8BAF5-5596-4D4C-9ECF-F37BF972A5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F657FA28-6315-4807-8435-02F3AA646B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intents" sheetId="1" r:id="rId1"/>
@@ -20,126 +20,137 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>capabilities</t>
+  </si>
+  <si>
+    <t>thanks</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Intent</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>book, reservation, reserve, booking, make a reservation</t>
+  </si>
+  <si>
+    <t>positive_responses</t>
+  </si>
+  <si>
+    <t>negative_responses</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>AskAboutRestaurant</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
   <si>
     <t>exit</t>
-  </si>
-  <si>
-    <t>cancel, exit, quit, bye, goodbye</t>
-  </si>
-  <si>
-    <t>book</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wellbeing_query</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>change</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Response</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Goodbye! ,Wishing you a wonderful day!, Goodbye see you soon!, Take care hope to see you again!</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Let's begin with your reservation., Let's get your reservation started!, I can help you make a reservation, let's proceed!</t>
+  </si>
+  <si>
+    <t>Hello!, How may I assist you?, Hi there! What can I do for you today?, Greetings! How can I help you?</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>I'm just a chatbot but I'm doing great thank you!, I'm functioning well thanks for asking!, As a chatbot  I don’t have feelings  but I’m here to help!</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>I can assist you with booking a table and answer questions., Type 'book' to make a reservation or ask me anything and I’ll do my best to answer!,Not much just waiting to assist you!, Just here and ready to help!, I’m here feel free to ask me anything!</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>You're very welcome! Anything else I can help with?, Glad to be of assistance!, It’s my pleasure, feel free to ask more questions!</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glad to be of assistance!</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>I am sorry for that</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hello, hi, greetings, hey there,hey</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>what can you do, what can you help with, assist, help me,features</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>change, change my name, update, update my name,a different name</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>restaurant, location, place, restaurant name, menu, food, dish, items, address, where, hours, operating hours, opening hours, opening time, offers, special offers, promotions, discounts,serving dinner,restaurant's schedule</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cancel, exit, quit, bye, goodbye,close,shut down,no more,end,no more,log off</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>thank you, thanks, appreciate it,grateful,owe you,thankful</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>n, no, nah, nope,don't agree,wrong,not sure,not interested,not up for it</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>hello</t>
-  </si>
-  <si>
-    <t>wellbeing_query</t>
-  </si>
-  <si>
-    <t>capabilities</t>
-  </si>
-  <si>
-    <t>small_talk</t>
-  </si>
-  <si>
-    <t>thanks</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Intent</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Response</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>book, reservation, reserve, booking, make a reservation</t>
-  </si>
-  <si>
-    <t>Let's begin with your reservation., Let's get your reservation started!, I can help you make a reservation, let's proceed!</t>
-  </si>
-  <si>
-    <t>I can assist you with booking a table and answer questions., Type 'book' to make a reservation or ask me anything and I’ll do my best to answer!</t>
-  </si>
-  <si>
-    <t>how are you, how's it going, how are you feeling, how’s your day</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>what can you do, what can you help with, assist, help me</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hello, hi, greetings, hey there</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>You're very welcome! Anything else I can help with?, Glad to be of assistance!, It’s my pleasure, feel free to ask more questions!</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Not much just waiting to assist you!, Just here and ready to help!, I’m here feel free to ask me anything!</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>I'm just a chatbot but I'm doing great thank you!, I'm functioning well thanks for asking!, As a chatbot  I don’t have feelings  but I’m here to help!</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hello!, How may I assist you?, Hi there! What can I do for you today?, Greetings! How can I help you?</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Goodbye! ,Wishing you a wonderful day!, Goodbye see you soon!, Take care hope to see you again!</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>positive_responses</t>
-  </si>
-  <si>
-    <t>negative_responses</t>
-  </si>
-  <si>
-    <t>Glad to be of assistance!</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>I am sorry for that</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>n, no, nah, nope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y, yes, okay, confirm, ok, yeah, sure </t>
-  </si>
-  <si>
-    <t>thank you, thanks, I appreciate it</t>
-  </si>
-  <si>
-    <t>what's up, what’s happening, what’s new, whats up</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>change</t>
-  </si>
-  <si>
-    <t>change, change my name, update, update my name</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>time, current time, what time is it, can you tell me the time, do you know the current time</t>
-  </si>
-  <si>
-    <t>my name, do you remember my name, do you know my name, who am i, tell me who am i, call my name, what's my name, call me, my name is</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>my name, do you remember my name, do you know my name,  who am i, call my name, what's my name, call me, my name is</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>time, current time, what time is it, do you know the current time,check the time,early or late.what hour</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>how are you, how's it going, how’s your day,what's up, what’s happening, what’s new, whats up</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>y, yes, okay, confirm, ok, yeah, sure ,no problem,correct,grateful</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -150,7 +161,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -158,7 +169,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -166,7 +177,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="等线 Light"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -175,7 +186,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -184,7 +195,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -193,7 +204,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -201,7 +212,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -209,7 +220,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -217,7 +228,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -225,7 +236,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -234,7 +245,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -243,7 +254,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -251,7 +262,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -260,7 +271,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -268,7 +279,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -277,7 +288,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -286,7 +297,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -294,14 +305,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -739,48 +750,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -796,9 +807,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -836,7 +847,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -942,7 +953,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1084,7 +1095,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1094,138 +1105,135 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="256" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
-    <col min="2" max="2" width="54.5" customWidth="1"/>
-    <col min="3" max="3" width="206.1640625" customWidth="1"/>
+    <col min="1" max="1" width="51.25" customWidth="1"/>
+    <col min="2" max="2" width="170.375" customWidth="1"/>
+    <col min="3" max="3" width="206.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>23</v>
+      <c r="A10" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>32</v>
@@ -1233,10 +1241,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>